<commit_message>
tedarikçi mail gönder formu
</commit_message>
<xml_diff>
--- a/IhalematikPro/EmailFile/SentFile/Entes Elektrik-11.03.2018-Malzeme_Fiyat_Listesi.xlsx
+++ b/IhalematikPro/EmailFile/SentFile/Entes Elektrik-11.03.2018-Malzeme_Fiyat_Listesi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>SIRA</t>
   </si>
@@ -72,103 +72,22 @@
     <t>Entes Elektrik</t>
   </si>
   <si>
-    <t>Ağ Görüntü Kayıt Cihazı (NVR)</t>
+    <t>GENERAL 11KW 0 KONTAKTÖR</t>
   </si>
   <si>
-    <t>adet</t>
+    <t>Adet</t>
   </si>
   <si>
-    <t>Dış Ortam Sabit Box/Bullet Tipi Kamera (Kamera Muhafazası ve Infrared LED Projektör dahil)</t>
+    <t>4X16+10 ALÜMİNYUM KABLO</t>
   </si>
   <si>
-    <t>Hareketli (Speed Dome) Kamera</t>
+    <t>DILM225-S/22 KONTAKTÖR 110KW</t>
   </si>
   <si>
-    <t>Saha Anahtarı (TİP1)</t>
+    <t>C63-3X63A GRUP OTOMAT</t>
   </si>
   <si>
-    <t>İç ortam ağ anahtarı (TİP2)</t>
-  </si>
-  <si>
-    <t>Klima 8 BTU İNVERTIR</t>
-  </si>
-  <si>
-    <t>Operatör Bilgisayarı</t>
-  </si>
-  <si>
-    <t>Operatör Bilgisayarı Monitörü</t>
-  </si>
-  <si>
-    <t>Rack Kabin</t>
-  </si>
-  <si>
-    <t>Saha Dolabı</t>
-  </si>
-  <si>
-    <t>1 KVA Kesintisiz Güç Kaynağı (UPS)</t>
-  </si>
-  <si>
-    <t>5 KVA Kesintisiz Güç Kaynağı (UPS)</t>
-  </si>
-  <si>
-    <t>Dıs Mahal Kazısı Toprak</t>
-  </si>
-  <si>
-    <t>metre</t>
-  </si>
-  <si>
-    <t>Dıs Mahal Kazısı Asfalt/Beton</t>
-  </si>
-  <si>
-    <t>Menhol</t>
-  </si>
-  <si>
-    <t>Dış Ortam Koruyucu Boruları (Koruge Boru)</t>
-  </si>
-  <si>
-    <t>Enerji Besleme Kabloları</t>
-  </si>
-  <si>
-    <t>Cat 6A UTP Kablo</t>
-  </si>
-  <si>
-    <t>Cat6A Patch Panel</t>
-  </si>
-  <si>
-    <t>Fiber Patch Panel (Cord)</t>
-  </si>
-  <si>
-    <t>Fiber Optik Pigtail ve kablosu</t>
-  </si>
-  <si>
-    <t>Fiber Optik Ek Kutu</t>
-  </si>
-  <si>
-    <t>Fiber Optik Atlama Kablosu</t>
-  </si>
-  <si>
-    <t>SM Fiber Optik (F/O) Kablo</t>
-  </si>
-  <si>
-    <t>Elektrik Panosu</t>
-  </si>
-  <si>
-    <t>Anahtarlı Otomatik Sigorta</t>
-  </si>
-  <si>
-    <t>Prizler</t>
-  </si>
-  <si>
-    <t>Kablo Kanaletleri</t>
-  </si>
-  <si>
-    <t>Delikli Tip Kapaklı Metal Kablo Kanalı</t>
-  </si>
-  <si>
-    <t>Direk ve Sabitleme (8 Metre)</t>
-  </si>
-  <si>
-    <t>Direk Üzeri Uzatma Aparatı</t>
+    <t>4X1,5 NYM KABLO</t>
   </si>
 </sst>
 </file>
@@ -1036,13 +955,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E8" s="14">
         <v>1</v>
@@ -1054,20 +973,20 @@
         <v>18</v>
       </c>
       <c r="H8" s="15">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="E9" s="18">
         <v>2</v>
@@ -1079,20 +998,20 @@
         <v>18</v>
       </c>
       <c r="H9" s="19">
-        <v>768</v>
+        <v>200</v>
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="E10" s="18">
         <v>3</v>
@@ -1104,20 +1023,20 @@
         <v>18</v>
       </c>
       <c r="H10" s="19">
-        <v>34</v>
+        <v>300</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E11" s="18">
         <v>4</v>
@@ -1129,20 +1048,20 @@
         <v>18</v>
       </c>
       <c r="H11" s="19">
-        <v>109</v>
+        <v>400</v>
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E12" s="18">
         <v>5</v>
@@ -1154,662 +1073,220 @@
         <v>18</v>
       </c>
       <c r="H12" s="19">
-        <v>47</v>
+        <v>500</v>
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>16</v>
-      </c>
-      <c r="E13" s="18">
-        <v>6</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="19">
-        <v>37</v>
-      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="20"/>
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>17</v>
-      </c>
-      <c r="E14" s="18">
-        <v>7</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="19">
-        <v>42</v>
-      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
       <c r="I14" s="20"/>
       <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>18</v>
-      </c>
-      <c r="E15" s="18">
-        <v>8</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="19">
-        <v>42</v>
-      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="20"/>
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>19</v>
-      </c>
-      <c r="E16" s="18">
-        <v>9</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="19">
-        <v>48</v>
-      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
       <c r="I16" s="20"/>
       <c r="J16" s="21"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>20</v>
-      </c>
-      <c r="E17" s="18">
-        <v>10</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="19">
-        <v>100</v>
-      </c>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="20"/>
       <c r="J17" s="21"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B18">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>21</v>
-      </c>
-      <c r="E18" s="18">
-        <v>11</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="19">
-        <v>108</v>
-      </c>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="20"/>
       <c r="J18" s="21"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>22</v>
-      </c>
-      <c r="E19" s="18">
-        <v>12</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="19">
-        <v>40</v>
-      </c>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="20"/>
       <c r="J19" s="21"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>23</v>
-      </c>
-      <c r="E20" s="18">
-        <v>13</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="19">
-        <v>2570</v>
-      </c>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="20"/>
       <c r="J20" s="21"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>24</v>
-      </c>
-      <c r="E21" s="18">
-        <v>14</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="19">
-        <v>8390</v>
-      </c>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
       <c r="I21" s="20"/>
       <c r="J21" s="21"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>25</v>
-      </c>
-      <c r="E22" s="18">
-        <v>15</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="19">
-        <v>307</v>
-      </c>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
       <c r="I22" s="20"/>
       <c r="J22" s="21"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>26</v>
-      </c>
-      <c r="E23" s="18">
-        <v>16</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="19">
-        <v>21860</v>
-      </c>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E23" s="18"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
       <c r="I23" s="20"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>27</v>
-      </c>
-      <c r="E24" s="18">
-        <v>17</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H24" s="19">
-        <v>24990</v>
-      </c>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
       <c r="I24" s="20"/>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>28</v>
-      </c>
-      <c r="E25" s="18">
-        <v>18</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="19">
-        <v>32960</v>
-      </c>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E25" s="18"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
       <c r="I25" s="20"/>
       <c r="J25" s="21"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B26">
-        <v>3</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <v>29</v>
-      </c>
-      <c r="E26" s="18">
-        <v>19</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="19">
-        <v>145</v>
-      </c>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="20"/>
       <c r="J26" s="21"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>30</v>
-      </c>
-      <c r="E27" s="18">
-        <v>20</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="19">
-        <v>145</v>
-      </c>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="20"/>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <v>31</v>
-      </c>
-      <c r="E28" s="18">
-        <v>21</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="19">
-        <v>305</v>
-      </c>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="20"/>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>32</v>
-      </c>
-      <c r="E29" s="18">
-        <v>22</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="19">
-        <v>54</v>
-      </c>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E29" s="18"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="20"/>
       <c r="J29" s="21"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>33</v>
-      </c>
-      <c r="E30" s="18">
-        <v>23</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="19">
-        <v>306</v>
-      </c>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
       <c r="I30" s="20"/>
       <c r="J30" s="21"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>34</v>
-      </c>
-      <c r="E31" s="18">
-        <v>24</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="19">
-        <v>12500</v>
-      </c>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E31" s="18"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="20"/>
       <c r="J31" s="21"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>35</v>
-      </c>
-      <c r="E32" s="18">
-        <v>25</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="19">
-        <v>40</v>
-      </c>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
       <c r="I32" s="20"/>
       <c r="J32" s="21"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>36</v>
-      </c>
-      <c r="E33" s="18">
-        <v>26</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="19">
-        <v>430</v>
-      </c>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E33" s="18"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
       <c r="I33" s="20"/>
       <c r="J33" s="21"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>37</v>
-      </c>
-      <c r="E34" s="18">
-        <v>27</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="19">
-        <v>215</v>
-      </c>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
       <c r="I34" s="20"/>
       <c r="J34" s="21"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>38</v>
-      </c>
-      <c r="E35" s="18">
-        <v>28</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H35" s="19">
-        <v>1450</v>
-      </c>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E35" s="18"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
       <c r="I35" s="20"/>
       <c r="J35" s="21"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36">
-        <v>39</v>
-      </c>
-      <c r="E36" s="18">
-        <v>29</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H36" s="19">
-        <v>1120</v>
-      </c>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E36" s="18"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
       <c r="I36" s="20"/>
       <c r="J36" s="21"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>40</v>
-      </c>
-      <c r="E37" s="18">
-        <v>30</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="19">
-        <v>176</v>
-      </c>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E37" s="18"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
       <c r="I37" s="20"/>
       <c r="J37" s="21"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>41</v>
-      </c>
-      <c r="E38" s="18">
-        <v>31</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="19">
-        <v>38</v>
-      </c>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.35">
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
       <c r="I38" s="20"/>
       <c r="J38" s="21"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E39" s="18"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
@@ -1817,7 +1294,7 @@
       <c r="I39" s="20"/>
       <c r="J39" s="21"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E40" s="18"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
@@ -1825,7 +1302,7 @@
       <c r="I40" s="20"/>
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E41" s="18"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -1833,7 +1310,7 @@
       <c r="I41" s="20"/>
       <c r="J41" s="21"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -1841,7 +1318,7 @@
       <c r="I42" s="20"/>
       <c r="J42" s="21"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E43" s="18"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
@@ -1849,7 +1326,7 @@
       <c r="I43" s="20"/>
       <c r="J43" s="21"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E44" s="18"/>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
@@ -1857,7 +1334,7 @@
       <c r="I44" s="20"/>
       <c r="J44" s="21"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E45" s="18"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
@@ -1865,7 +1342,7 @@
       <c r="I45" s="20"/>
       <c r="J45" s="21"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E46" s="18"/>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -1873,7 +1350,7 @@
       <c r="I46" s="20"/>
       <c r="J46" s="21"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E47" s="18"/>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -1881,7 +1358,7 @@
       <c r="I47" s="20"/>
       <c r="J47" s="21"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:10" x14ac:dyDescent="0.35">
       <c r="E48" s="18"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>

</xml_diff>